<commit_message>
modifs sur scripts conversions JSON
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\quiz maxime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\quiz\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DF1971-0A47-4C9D-824C-ADCA7150FC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD8117F-40BA-4E69-B7E0-AB3A45A9A026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-16308" windowWidth="29016" windowHeight="15696" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="1" r:id="rId1"/>
+    <sheet name="Infos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="146">
   <si>
     <t>id</t>
   </si>
@@ -71,404 +94,416 @@
     <t>Combien de serveurs gérons-nous dans notre infrastructure ?</t>
   </si>
   <si>
+    <t>Environ 11</t>
+  </si>
+  <si>
+    <t>Environ 20</t>
+  </si>
+  <si>
+    <t>Nous n'avons pas de serveurs</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>Parmi les types de serveurs suivants, lequel est principalement utilisé pour stocker des fichiers ?</t>
+  </si>
+  <si>
+    <t>Serveur AD</t>
+  </si>
+  <si>
+    <t>Serveur NAS</t>
+  </si>
+  <si>
+    <t>Serveur de Sauvegarde</t>
+  </si>
+  <si>
+    <t>Serveur TSE/RDS</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>À quoi sert principalement un serveur TSE/RDS ?</t>
+  </si>
+  <si>
+    <t>À gérer les identités des utilisateurs</t>
+  </si>
+  <si>
+    <t>À stocker les sauvegardes de données</t>
+  </si>
+  <si>
+    <t>À permettre l'accès à des applications et des bureaux à distance</t>
+  </si>
+  <si>
+    <t>À héberger le site web de l'entreprise</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>Quel système d'exploitation est utilisé sur nos serveurs principaux ?</t>
+  </si>
+  <si>
+    <t>Windows 10 Professionnel</t>
+  </si>
+  <si>
+    <t>Windows Server 2022 Datacenter</t>
+  </si>
+  <si>
+    <t>Linux Ubuntu</t>
+  </si>
+  <si>
+    <t>macOS Server</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>Nos Postes de Travail</t>
+  </si>
+  <si>
+    <t>Combien de postes de travail (PC fixes et portables) sont en service dans notre entreprise ?</t>
+  </si>
+  <si>
+    <t>Moins de 100</t>
+  </si>
+  <si>
+    <t>Environ 250</t>
+  </si>
+  <si>
+    <t>Plus de 500</t>
+  </si>
+  <si>
+    <t>Le nombre varie constamment</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>Quels systèmes d'exploitation équipent la majorité de nos postes de travail ?</t>
+  </si>
+  <si>
+    <t>Principalement macOS</t>
+  </si>
+  <si>
+    <t>Uniquement Windows 7</t>
+  </si>
+  <si>
+    <t>Windows 10 et 11 Professionnel</t>
+  </si>
+  <si>
+    <t>Des versions Entreprise de Windows</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>Qu'est-ce qu'un compte utilisateur sur votre ordinateur ou dans le réseau de l'entreprise ?</t>
+  </si>
+  <si>
+    <t>Un programme pour faire des calculs</t>
+  </si>
+  <si>
+    <t>Un identifiant unique avec mot de passe qui donne accès à vos documents, logiciels et paramètres</t>
+  </si>
+  <si>
+    <t>Un service de messagerie instantanée</t>
+  </si>
+  <si>
+    <t>Le nom de l'ordinateur</t>
+  </si>
+  <si>
+    <t>q8</t>
+  </si>
+  <si>
+    <t>Comment changer son mot de passe Windows ?</t>
+  </si>
+  <si>
+    <t>Redémarrer l'ordinateur</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + Suppr puis Modifier un mot de passe</t>
+  </si>
+  <si>
+    <t>Aller dans le Panneau de configuration</t>
+  </si>
+  <si>
+    <t>Les réponses B et C sont correctes</t>
+  </si>
+  <si>
+    <t>q9</t>
+  </si>
+  <si>
+    <t>Accessoires et Windows</t>
+  </si>
+  <si>
+    <t>Quel outil intégré à Windows permet de réaliser rapidement une capture d'écran ?</t>
+  </si>
+  <si>
+    <t>Paint</t>
+  </si>
+  <si>
+    <t>L'Outil Capture d'écran</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Le Gestionnaire des tâches</t>
+  </si>
+  <si>
+    <t>q10</t>
+  </si>
+  <si>
+    <t>Pourquoi est-il important d'effectuer les mises à jour de Windows et des pilotes ?</t>
+  </si>
+  <si>
+    <t>Pour ralentir l'ordinateur</t>
+  </si>
+  <si>
+    <t>Pour améliorer la sécurité et la stabilité</t>
+  </si>
+  <si>
+    <t>Pour changer l'interface graphique</t>
+  </si>
+  <si>
+    <t>Pour consommer plus d'énergie</t>
+  </si>
+  <si>
+    <t>q11</t>
+  </si>
+  <si>
+    <t>Où chercher rapidement une application ou un fichier sur votre PC ?</t>
+  </si>
+  <si>
+    <t>Le Bureau</t>
+  </si>
+  <si>
+    <t>La barre des tâches</t>
+  </si>
+  <si>
+    <t>La barre de recherche</t>
+  </si>
+  <si>
+    <t>q12</t>
+  </si>
+  <si>
+    <t>Quel est le raccourci clavier pour copier un élément sélectionné ?</t>
+  </si>
+  <si>
+    <t>Ctrl + X</t>
+  </si>
+  <si>
+    <t>Ctrl + V</t>
+  </si>
+  <si>
+    <t>Ctrl + C</t>
+  </si>
+  <si>
+    <t>Ctrl + Z</t>
+  </si>
+  <si>
+    <t>q13</t>
+  </si>
+  <si>
+    <t>Quel est le raccourci clavier pour basculer entre plusieurs fenêtres ouvertes ?</t>
+  </si>
+  <si>
+    <t>Alt + F4</t>
+  </si>
+  <si>
+    <t>Ctrl + S</t>
+  </si>
+  <si>
+    <t>Alt + Tab</t>
+  </si>
+  <si>
+    <t>Windows + D</t>
+  </si>
+  <si>
+    <t>q14</t>
+  </si>
+  <si>
+    <t>Comment fermer une application qui ne répond plus ?</t>
+  </si>
+  <si>
+    <t>Utiliser Ctrl + Alt + Suppr ou clic droit sur la barre des tâches puis le Gestionnaire des tâches</t>
+  </si>
+  <si>
+    <t>Attendre qu'elle se ferme toute seule</t>
+  </si>
+  <si>
+    <t>Se déconnecter et se reconnecter</t>
+  </si>
+  <si>
+    <t>q15</t>
+  </si>
+  <si>
+    <t>Pourquoi faut-il fermer ses applications et éteindre son ordinateur le soir ?</t>
+  </si>
+  <si>
+    <t>Eviter une surchauffe de l’ordinateur</t>
+  </si>
+  <si>
+    <t>Empêcher le piratage informatique</t>
+  </si>
+  <si>
+    <t>Permettre une sauvegarde achevée</t>
+  </si>
+  <si>
+    <t>Je ne sais pas</t>
+  </si>
+  <si>
+    <t>q16</t>
+  </si>
+  <si>
+    <t>Imprimantes</t>
+  </si>
+  <si>
+    <t>Nos imprimantes permettent-elles de scanner des documents ?</t>
+  </si>
+  <si>
+    <t>Oui, toutes</t>
+  </si>
+  <si>
+    <t>Non, aucune</t>
+  </si>
+  <si>
+    <t>Seulement quelques modèles</t>
+  </si>
+  <si>
+    <t>q17</t>
+  </si>
+  <si>
+    <t>Fonctionnalité pratique du scan pour partager des documents ?</t>
+  </si>
+  <si>
+    <t>Scan to Music</t>
+  </si>
+  <si>
+    <t>Scan to Mail/Folder</t>
+  </si>
+  <si>
+    <t>Scan to Game</t>
+  </si>
+  <si>
+    <t>Scan to Print</t>
+  </si>
+  <si>
+    <t>q18</t>
+  </si>
+  <si>
+    <t>Fréquence d'utilisation des imprimantes dans les groupes de travail ?</t>
+  </si>
+  <si>
+    <t>Très faible</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>Très élevée</t>
+  </si>
+  <si>
+    <t>Je n'imprime jamais</t>
+  </si>
+  <si>
+    <t>q19</t>
+  </si>
+  <si>
+    <t>Téléphonie</t>
+  </si>
+  <si>
+    <t>Qu'est-ce qu'un numéro SDA ?</t>
+  </si>
+  <si>
+    <t>Numéro d'urgence</t>
+  </si>
+  <si>
+    <t>Numéro direct attribué à un poste ou service</t>
+  </si>
+  <si>
+    <t>Numéro de fax</t>
+  </si>
+  <si>
+    <t>Numéro de mobile professionnel</t>
+  </si>
+  <si>
+    <t>q20</t>
+  </si>
+  <si>
+    <t>Combien de téléphones professionnels en service ?</t>
+  </si>
+  <si>
+    <t>Environ 224</t>
+  </si>
+  <si>
+    <t>Plus de 300</t>
+  </si>
+  <si>
+    <t>Aucun</t>
+  </si>
+  <si>
+    <t>q21</t>
+  </si>
+  <si>
+    <t>Cybersécurité</t>
+  </si>
+  <si>
+    <t>Est-il recommandé d’enregistrer vos mots de passe dans le navigateur ?</t>
+  </si>
+  <si>
+    <t>Oui, c'est très pratique et sûr</t>
+  </si>
+  <si>
+    <t>Oui, si l'ordinateur est protégé par mot de passe</t>
+  </si>
+  <si>
+    <t>Non, ce n'est pas recommandé pour des raisons de sécurité</t>
+  </si>
+  <si>
+    <t>Cela dépend du site</t>
+  </si>
+  <si>
+    <t>q22</t>
+  </si>
+  <si>
+    <t>Que faire avec un mail suspect contenant un lien ou une pièce jointe ?</t>
+  </si>
+  <si>
+    <t>Ouvrir immédiatement</t>
+  </si>
+  <si>
+    <t>Transférer à tous vos collègues</t>
+  </si>
+  <si>
+    <t>Le signaler à votre support informatique et le supprimer</t>
+  </si>
+  <si>
+    <t>Le marquer comme spam et l'ignorer</t>
+  </si>
+  <si>
+    <t>Ce quiz a été conçu pour tester vos connaissances tout en vous amusant.</t>
+  </si>
+  <si>
     <t>Environ 5</t>
   </si>
   <si>
-    <t>Environ 11</t>
-  </si>
-  <si>
-    <t>Environ 20</t>
-  </si>
-  <si>
-    <t>Nous n'avons pas de serveurs</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>Parmi les types de serveurs suivants, lequel est principalement utilisé pour stocker des fichiers ?</t>
-  </si>
-  <si>
-    <t>Serveur AD</t>
-  </si>
-  <si>
-    <t>Serveur NAS</t>
-  </si>
-  <si>
-    <t>Serveur de Sauvegarde</t>
-  </si>
-  <si>
-    <t>Serveur TSE/RDS</t>
-  </si>
-  <si>
-    <t>q3</t>
-  </si>
-  <si>
-    <t>À quoi sert principalement un serveur TSE/RDS ?</t>
-  </si>
-  <si>
-    <t>À gérer les identités des utilisateurs</t>
-  </si>
-  <si>
-    <t>À stocker les sauvegardes de données</t>
-  </si>
-  <si>
-    <t>À permettre l'accès à des applications et des bureaux à distance</t>
-  </si>
-  <si>
-    <t>À héberger le site web de l'entreprise</t>
-  </si>
-  <si>
-    <t>q4</t>
-  </si>
-  <si>
-    <t>Quel système d'exploitation est utilisé sur nos serveurs principaux ?</t>
-  </si>
-  <si>
-    <t>Windows 10 Professionnel</t>
-  </si>
-  <si>
-    <t>Windows Server 2022 Datacenter</t>
-  </si>
-  <si>
-    <t>Linux Ubuntu</t>
-  </si>
-  <si>
-    <t>macOS Server</t>
-  </si>
-  <si>
-    <t>q5</t>
-  </si>
-  <si>
-    <t>Nos Postes de Travail</t>
-  </si>
-  <si>
-    <t>Combien de postes de travail (PC fixes et portables) sont en service dans notre entreprise ?</t>
-  </si>
-  <si>
-    <t>Moins de 100</t>
-  </si>
-  <si>
-    <t>Environ 250</t>
-  </si>
-  <si>
-    <t>Plus de 500</t>
-  </si>
-  <si>
-    <t>Le nombre varie constamment</t>
-  </si>
-  <si>
-    <t>q6</t>
-  </si>
-  <si>
-    <t>Quels systèmes d'exploitation équipent la majorité de nos postes de travail ?</t>
-  </si>
-  <si>
-    <t>Principalement macOS</t>
-  </si>
-  <si>
-    <t>Uniquement Windows 7</t>
-  </si>
-  <si>
-    <t>Windows 10 et 11 Professionnel</t>
-  </si>
-  <si>
-    <t>Des versions Entreprise de Windows</t>
-  </si>
-  <si>
-    <t>q7</t>
-  </si>
-  <si>
-    <t>Qu'est-ce qu'un compte utilisateur sur votre ordinateur ou dans le réseau de l'entreprise ?</t>
-  </si>
-  <si>
-    <t>Un programme pour faire des calculs</t>
-  </si>
-  <si>
-    <t>Un identifiant unique avec mot de passe qui donne accès à vos documents, logiciels et paramètres</t>
-  </si>
-  <si>
-    <t>Un service de messagerie instantanée</t>
-  </si>
-  <si>
-    <t>Le nom de l'ordinateur</t>
-  </si>
-  <si>
-    <t>q8</t>
-  </si>
-  <si>
-    <t>Comment changer son mot de passe Windows ?</t>
-  </si>
-  <si>
-    <t>Redémarrer l'ordinateur</t>
-  </si>
-  <si>
-    <t>Ctrl + Alt + Suppr puis Modifier un mot de passe</t>
-  </si>
-  <si>
-    <t>Aller dans le Panneau de configuration</t>
-  </si>
-  <si>
-    <t>Les réponses B et C sont correctes</t>
-  </si>
-  <si>
-    <t>q9</t>
-  </si>
-  <si>
-    <t>Accessoires et Windows</t>
-  </si>
-  <si>
-    <t>Quel outil intégré à Windows permet de réaliser rapidement une capture d'écran ?</t>
-  </si>
-  <si>
-    <t>Paint</t>
-  </si>
-  <si>
-    <t>L'Outil Capture d'écran</t>
-  </si>
-  <si>
-    <t>Word</t>
-  </si>
-  <si>
-    <t>Le Gestionnaire des tâches</t>
-  </si>
-  <si>
-    <t>q10</t>
-  </si>
-  <si>
-    <t>Pourquoi est-il important d'effectuer les mises à jour de Windows et des pilotes ?</t>
-  </si>
-  <si>
-    <t>Pour ralentir l'ordinateur</t>
-  </si>
-  <si>
-    <t>Pour améliorer la sécurité et la stabilité</t>
-  </si>
-  <si>
-    <t>Pour changer l'interface graphique</t>
-  </si>
-  <si>
-    <t>Pour consommer plus d'énergie</t>
-  </si>
-  <si>
-    <t>q11</t>
-  </si>
-  <si>
-    <t>Où chercher rapidement une application ou un fichier sur votre PC ?</t>
-  </si>
-  <si>
-    <t>Le Bureau</t>
-  </si>
-  <si>
-    <t>La barre des tâches</t>
-  </si>
-  <si>
-    <t>La barre de recherche</t>
-  </si>
-  <si>
-    <t>q12</t>
-  </si>
-  <si>
-    <t>Quel est le raccourci clavier pour copier un élément sélectionné ?</t>
-  </si>
-  <si>
-    <t>Ctrl + X</t>
-  </si>
-  <si>
-    <t>Ctrl + V</t>
-  </si>
-  <si>
-    <t>Ctrl + C</t>
-  </si>
-  <si>
-    <t>Ctrl + Z</t>
-  </si>
-  <si>
-    <t>q13</t>
-  </si>
-  <si>
-    <t>Quel est le raccourci clavier pour basculer entre plusieurs fenêtres ouvertes ?</t>
-  </si>
-  <si>
-    <t>Alt + F4</t>
-  </si>
-  <si>
-    <t>Ctrl + S</t>
-  </si>
-  <si>
-    <t>Alt + Tab</t>
-  </si>
-  <si>
-    <t>Windows + D</t>
-  </si>
-  <si>
-    <t>q14</t>
-  </si>
-  <si>
-    <t>Comment fermer une application qui ne répond plus ?</t>
-  </si>
-  <si>
-    <t>Utiliser Ctrl + Alt + Suppr ou clic droit sur la barre des tâches puis le Gestionnaire des tâches</t>
-  </si>
-  <si>
-    <t>Attendre qu'elle se ferme toute seule</t>
-  </si>
-  <si>
-    <t>Se déconnecter et se reconnecter</t>
-  </si>
-  <si>
-    <t>q15</t>
-  </si>
-  <si>
-    <t>Pourquoi faut-il fermer ses applications et éteindre son ordinateur le soir ?</t>
-  </si>
-  <si>
-    <t>Eviter une surchauffe de l’ordinateur</t>
-  </si>
-  <si>
-    <t>Empêcher le piratage informatique</t>
-  </si>
-  <si>
-    <t>Permettre une sauvegarde achevée</t>
-  </si>
-  <si>
-    <t>Je ne sais pas</t>
-  </si>
-  <si>
-    <t>q16</t>
-  </si>
-  <si>
-    <t>Imprimantes</t>
-  </si>
-  <si>
-    <t>Nos imprimantes permettent-elles de scanner des documents ?</t>
-  </si>
-  <si>
-    <t>Oui, toutes</t>
-  </si>
-  <si>
-    <t>Non, aucune</t>
-  </si>
-  <si>
-    <t>Seulement quelques modèles</t>
-  </si>
-  <si>
-    <t>q17</t>
-  </si>
-  <si>
-    <t>Fonctionnalité pratique du scan pour partager des documents ?</t>
-  </si>
-  <si>
-    <t>Scan to Music</t>
-  </si>
-  <si>
-    <t>Scan to Mail/Folder</t>
-  </si>
-  <si>
-    <t>Scan to Game</t>
-  </si>
-  <si>
-    <t>Scan to Print</t>
-  </si>
-  <si>
-    <t>q18</t>
-  </si>
-  <si>
-    <t>Fréquence d'utilisation des imprimantes dans les groupes de travail ?</t>
-  </si>
-  <si>
-    <t>Très faible</t>
-  </si>
-  <si>
-    <t>Moyenne</t>
-  </si>
-  <si>
-    <t>Très élevée</t>
-  </si>
-  <si>
-    <t>Je n'imprime jamais</t>
-  </si>
-  <si>
-    <t>q19</t>
-  </si>
-  <si>
-    <t>Téléphonie</t>
-  </si>
-  <si>
-    <t>Qu'est-ce qu'un numéro SDA ?</t>
-  </si>
-  <si>
-    <t>Numéro d'urgence</t>
-  </si>
-  <si>
-    <t>Numéro direct attribué à un poste ou service</t>
-  </si>
-  <si>
-    <t>Numéro de fax</t>
-  </si>
-  <si>
-    <t>Numéro de mobile professionnel</t>
-  </si>
-  <si>
-    <t>q20</t>
-  </si>
-  <si>
-    <t>Combien de téléphones professionnels en service ?</t>
-  </si>
-  <si>
-    <t>Environ 224</t>
-  </si>
-  <si>
-    <t>Plus de 300</t>
-  </si>
-  <si>
-    <t>Aucun</t>
-  </si>
-  <si>
-    <t>q21</t>
-  </si>
-  <si>
-    <t>Cybersécurité</t>
-  </si>
-  <si>
-    <t>Est-il recommandé d’enregistrer vos mots de passe dans le navigateur ?</t>
-  </si>
-  <si>
-    <t>Oui, c'est très pratique et sûr</t>
-  </si>
-  <si>
-    <t>Oui, si l'ordinateur est protégé par mot de passe</t>
-  </si>
-  <si>
-    <t>Non, ce n'est pas recommandé pour des raisons de sécurité</t>
-  </si>
-  <si>
-    <t>Cela dépend du site</t>
-  </si>
-  <si>
-    <t>q22</t>
-  </si>
-  <si>
-    <t>Que faire avec un mail suspect contenant un lien ou une pièce jointe ?</t>
-  </si>
-  <si>
-    <t>Ouvrir immédiatement</t>
-  </si>
-  <si>
-    <t>Transférer à tous vos collègues</t>
-  </si>
-  <si>
-    <t>Le signaler à votre support informatique et le supprimer</t>
-  </si>
-  <si>
-    <t>Le marquer comme spam et l'ignorer</t>
+    <t>n° dossier parents recherché en  remontant le chemin</t>
+  </si>
+  <si>
+    <t>Titre-principal</t>
+  </si>
+  <si>
+    <t>Description-projet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +523,11 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="4">
@@ -590,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -610,11 +650,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -634,6 +689,36 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -690,7 +775,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE4CB63C-D694-4DE3-88A4-07728370621A}" name="Tableau1" displayName="Tableau1" ref="A1:H24" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE4CB63C-D694-4DE3-88A4-07728370621A}" name="Tableau1" displayName="Tableau1" ref="A1:H24" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:H24" xr:uid="{EE4CB63C-D694-4DE3-88A4-07728370621A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FFB5F9E7-A700-48FD-AA03-972C23F32A05}" name="id"/>
@@ -703,6 +788,20 @@
     <tableColumn id="8" xr3:uid="{6D13C61C-F204-4223-AFC0-3EDC9F97F7CC}" name="correctAnswer"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{258CCCC3-C1DB-4FE2-8020-64213AE98A01}" name="Tableau2" displayName="Tableau2" ref="A1:C2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:C2" xr:uid="{258CCCC3-C1DB-4FE2-8020-64213AE98A01}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6D38A9E1-CBF1-4322-B635-142AB4FA62BC}" name="n° dossier parents recherché en  remontant le chemin" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{90084625-3FE1-47C2-9F8F-0ADA5DF285D0}" name="Titre-principal" dataDxfId="3">
+      <calculatedColumnFormula array="1">TRIM(MID(SUBSTITUTE(CELL("nomfichier",B2),"\",REPT(" ",100)),(LEN(CELL("nomfichier",B2))-LEN(SUBSTITUTE(CELL("nomfichier",B2),"\",""))-A2)*100+1,100))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{CC573614-EC2B-4D68-A6EE-DECC879AE40B}" name="Description-projet" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1025,11 +1124,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAFCBC0-23DF-41B8-8FAF-33727A29218D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.5546875" bestFit="1" customWidth="1"/>
@@ -1038,7 +1137,7 @@
     <col min="8" max="8" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1064,7 +1163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="28.8">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1075,562 +1174,562 @@
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="43.2">
       <c r="A3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.8">
       <c r="A5" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="43.2">
       <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8">
       <c r="A7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="43.2">
       <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.8">
       <c r="A9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8">
       <c r="A10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="28.8">
       <c r="A11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="28.8">
       <c r="A12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="G12" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28.8">
       <c r="A13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28.8">
       <c r="A14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="43.2">
       <c r="A15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="28.8">
       <c r="A16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="28.8">
       <c r="A17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>104</v>
-      </c>
       <c r="G17" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="28.8">
       <c r="A18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="28.8">
       <c r="A19" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="28.8">
       <c r="A21" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="28.8">
       <c r="A22" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>135</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="28.8">
       <c r="A23" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="E23" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="F23" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>5</v>
@@ -1653,4 +1752,56 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3203C7-98EA-4D95-946F-7FD39295760B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="24.5546875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="27" style="15" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="24.5546875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28.8">
+      <c r="A1" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="26.4">
+      <c r="A2" s="16">
+        <v>2</v>
+      </c>
+      <c r="B2" s="16" t="str" cm="1">
+        <f t="array" aca="1" ref="B2" ca="1">TRIM(MID(SUBSTITUTE(CELL("nomfichier",B2),"\",REPT(" ",100)),(LEN(CELL("nomfichier",B2))-LEN(SUBSTITUTE(CELL("nomfichier",B2),"\",""))-A2)*100+1,100))</f>
+        <v>quiz</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{AB0BACFE-C2FB-4A50-A489-D0AA9EFB7488}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modif autour de fichier excel
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\quiz\systeme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Questionnaire SI\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD8117F-40BA-4E69-B7E0-AB3A45A9A026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CADE97E-3688-437E-BCCD-1B076764624E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
+    <workbookView xWindow="384" yWindow="-15816" windowWidth="21600" windowHeight="11304" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1759,7 +1759,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5546875" defaultRowHeight="14.4"/>
@@ -1785,9 +1785,9 @@
       <c r="A2" s="16">
         <v>2</v>
       </c>
-      <c r="B2" s="16" t="str" cm="1">
+      <c r="B2" s="13" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">TRIM(MID(SUBSTITUTE(CELL("nomfichier",B2),"\",REPT(" ",100)),(LEN(CELL("nomfichier",B2))-LEN(SUBSTITUTE(CELL("nomfichier",B2),"\",""))-A2)*100+1,100))</f>
-        <v>quiz</v>
+        <v>Questionnaire SI</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
maj tableau excel via START
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Questionnaire SI\systeme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Quiz SI Metivier\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CADE97E-3688-437E-BCCD-1B076764624E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD6A7C0-0FE6-4393-906D-49B604CB4A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="-15816" windowWidth="21600" windowHeight="11304" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" s="13" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">TRIM(MID(SUBSTITUTE(CELL("nomfichier",B2),"\",REPT(" ",100)),(LEN(CELL("nomfichier",B2))-LEN(SUBSTITUTE(CELL("nomfichier",B2),"\",""))-A2)*100+1,100))</f>
-        <v>Questionnaire SI</v>
+        <v>Quiz SI Metivier</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
Mise à jour nom du quiz (dossier)
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Quiz SI Metivier\systeme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Quiz SI Methivier\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD6A7C0-0FE6-4393-906D-49B604CB4A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444AB2FC-E1DD-4009-909D-2B2683E704ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" s="13" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">TRIM(MID(SUBSTITUTE(CELL("nomfichier",B2),"\",REPT(" ",100)),(LEN(CELL("nomfichier",B2))-LEN(SUBSTITUTE(CELL("nomfichier",B2),"\",""))-A2)*100+1,100))</f>
-        <v>Quiz SI Metivier</v>
+        <v>Quiz SI Methivier</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
Excel : Ajout type graphique
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Quiz SI Methivier\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444AB2FC-E1DD-4009-909D-2B2683E704ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004F3D22-80EB-4609-B0D4-2E768B345F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="148">
   <si>
     <t>id</t>
   </si>
@@ -497,6 +497,12 @@
   </si>
   <si>
     <t>Description-projet</t>
+  </si>
+  <si>
+    <t>Graphique-resultats</t>
+  </si>
+  <si>
+    <t>Camenbert</t>
   </si>
 </sst>
 </file>
@@ -669,7 +675,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -689,24 +716,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -775,7 +784,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE4CB63C-D694-4DE3-88A4-07728370621A}" name="Tableau1" displayName="Tableau1" ref="A1:H24" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE4CB63C-D694-4DE3-88A4-07728370621A}" name="Tableau1" displayName="Tableau1" ref="A1:H24" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:H24" xr:uid="{EE4CB63C-D694-4DE3-88A4-07728370621A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FFB5F9E7-A700-48FD-AA03-972C23F32A05}" name="id"/>
@@ -792,14 +801,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{258CCCC3-C1DB-4FE2-8020-64213AE98A01}" name="Tableau2" displayName="Tableau2" ref="A1:C2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:C2" xr:uid="{258CCCC3-C1DB-4FE2-8020-64213AE98A01}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6D38A9E1-CBF1-4322-B635-142AB4FA62BC}" name="n° dossier parents recherché en  remontant le chemin" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{90084625-3FE1-47C2-9F8F-0ADA5DF285D0}" name="Titre-principal" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{258CCCC3-C1DB-4FE2-8020-64213AE98A01}" name="Tableau2" displayName="Tableau2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:D2" xr:uid="{258CCCC3-C1DB-4FE2-8020-64213AE98A01}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6D38A9E1-CBF1-4322-B635-142AB4FA62BC}" name="n° dossier parents recherché en  remontant le chemin" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{90084625-3FE1-47C2-9F8F-0ADA5DF285D0}" name="Titre-principal" dataDxfId="4">
       <calculatedColumnFormula array="1">TRIM(MID(SUBSTITUTE(CELL("nomfichier",B2),"\",REPT(" ",100)),(LEN(CELL("nomfichier",B2))-LEN(SUBSTITUTE(CELL("nomfichier",B2),"\",""))-A2)*100+1,100))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CC573614-EC2B-4D68-A6EE-DECC879AE40B}" name="Description-projet" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{CC573614-EC2B-4D68-A6EE-DECC879AE40B}" name="Description-projet" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D4F870EE-921B-4CDB-96F5-074B5A5499BD}" name="Graphique-resultats" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1737,10 +1747,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="ID déjà existante " error="!! ID déjà existante !! 👀" sqref="A1:A1048576" xr:uid="{72F7E06E-D266-4522-A123-47B12B66B093}">
@@ -1756,10 +1766,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3203C7-98EA-4D95-946F-7FD39295760B}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5546875" defaultRowHeight="14.4"/>
@@ -1770,7 +1780,7 @@
     <col min="4" max="16384" width="24.5546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8">
+    <row r="1" spans="1:4" ht="28.8">
       <c r="A1" s="13" t="s">
         <v>143</v>
       </c>
@@ -1780,8 +1790,11 @@
       <c r="C1" s="14" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="26.4">
+      <c r="D1" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="26.4">
       <c r="A2" s="16">
         <v>2</v>
       </c>
@@ -1792,11 +1805,17 @@
       <c r="C2" s="17" t="s">
         <v>141</v>
       </c>
+      <c r="D2" s="16" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{AB0BACFE-C2FB-4A50-A489-D0AA9EFB7488}">
       <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{CE53775F-3D12-4F66-9328-CE8DA2F82506}">
+      <formula1>"Camenbert, Diagramme, Jauge"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CONFIG.JSON : mise à jour scripte pour import type de Graphique-resultats
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Quiz SI Methivier\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004F3D22-80EB-4609-B0D4-2E768B345F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012B71C7-7811-496F-A0D2-D5A19CD26AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
@@ -677,6 +677,26 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -696,26 +716,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -808,8 +808,8 @@
     <tableColumn id="2" xr3:uid="{90084625-3FE1-47C2-9F8F-0ADA5DF285D0}" name="Titre-principal" dataDxfId="4">
       <calculatedColumnFormula array="1">TRIM(MID(SUBSTITUTE(CELL("nomfichier",B2),"\",REPT(" ",100)),(LEN(CELL("nomfichier",B2))-LEN(SUBSTITUTE(CELL("nomfichier",B2),"\",""))-A2)*100+1,100))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CC573614-EC2B-4D68-A6EE-DECC879AE40B}" name="Description-projet" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D4F870EE-921B-4CDB-96F5-074B5A5499BD}" name="Graphique-resultats" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{CC573614-EC2B-4D68-A6EE-DECC879AE40B}" name="Description-projet" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D4F870EE-921B-4CDB-96F5-074B5A5499BD}" name="Graphique-resultats" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1747,10 +1747,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="ID déjà existante " error="!! ID déjà existante !! 👀" sqref="A1:A1048576" xr:uid="{72F7E06E-D266-4522-A123-47B12B66B093}">
@@ -1769,7 +1769,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5546875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
RESULTATS : modifications diverses pour faire apparaitre les résultats en graphique
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Quiz SI Methivier\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012B71C7-7811-496F-A0D2-D5A19CD26AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE5BC21-FD77-47F1-8FE4-A4FAC372E11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
@@ -502,7 +502,7 @@
     <t>Graphique-resultats</t>
   </si>
   <si>
-    <t>Camenbert</t>
+    <t>camembert</t>
   </si>
 </sst>
 </file>
@@ -1769,7 +1769,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5546875" defaultRowHeight="14.4"/>
@@ -1815,7 +1815,7 @@
       <formula1>"1,2,3,4,5,6,7,8"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{CE53775F-3D12-4F66-9328-CE8DA2F82506}">
-      <formula1>"Camenbert, Diagramme, Jauge"</formula1>
+      <formula1>"camembert, diagramme, jauge"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modification graphique doc excel pour tests
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Quiz SI Methivier\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483BBF02-BF8F-4E1A-8DFE-2009EA9F7DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA6A3F2-1B01-466B-B1A7-F0AD37850325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
@@ -175,7 +175,7 @@
     <t>Graphique-resultats</t>
   </si>
   <si>
-    <t>jauge</t>
+    <t>diagramme</t>
   </si>
 </sst>
 </file>
@@ -974,7 +974,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5546875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
modif Excel pour test graphique
</commit_message>
<xml_diff>
--- a/systeme/Tableau-Questions.xlsx
+++ b/systeme/Tableau-Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheye\Documents\Quiz SI Methivier\systeme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA6A3F2-1B01-466B-B1A7-F0AD37850325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A95BB69-350E-4323-8E8C-1F17668BDBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4528FE17-A8AD-4311-A77A-5BA324C181ED}"/>
   </bookViews>
@@ -175,7 +175,7 @@
     <t>Graphique-resultats</t>
   </si>
   <si>
-    <t>diagramme</t>
+    <t>jauge</t>
   </si>
 </sst>
 </file>
@@ -974,7 +974,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5546875" defaultRowHeight="14.4"/>

</xml_diff>